<commit_message>
New feedback system and Reservation changes and fronted small corrections
</commit_message>
<xml_diff>
--- a/Backend/reservations.xlsx
+++ b/Backend/reservations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
   <si>
     <t>Priyank12</t>
   </si>
@@ -59,6 +59,48 @@
   </si>
   <si>
     <t>04:29</t>
+  </si>
+  <si>
+    <t>pitliyapriyank@gmail.com</t>
+  </si>
+  <si>
+    <t>2024-04-23</t>
+  </si>
+  <si>
+    <t>20:39</t>
+  </si>
+  <si>
+    <t>2024-04-24</t>
+  </si>
+  <si>
+    <t>19:02</t>
+  </si>
+  <si>
+    <t>gigi</t>
+  </si>
+  <si>
+    <t>2024-04-02</t>
+  </si>
+  <si>
+    <t>21:08</t>
+  </si>
+  <si>
+    <t>2024-04-16</t>
+  </si>
+  <si>
+    <t>23:20</t>
+  </si>
+  <si>
+    <t>2024-04-25</t>
+  </si>
+  <si>
+    <t>22:33</t>
+  </si>
+  <si>
+    <t>2024-04-14</t>
+  </si>
+  <si>
+    <t>19:34</t>
   </si>
 </sst>
 </file>
@@ -400,7 +442,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -630,6 +672,90 @@
         <v>14</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>